<commit_message>
LPF-970 - try a new template with the dev data
</commit_message>
<xml_diff>
--- a/src/main/resources/templateTweak.xlsx
+++ b/src/main/resources/templateTweak.xlsx
@@ -135,12 +135,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ dddd"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>

</xml_diff>